<commit_message>
Update inventory data pipeline and dashboard
</commit_message>
<xml_diff>
--- a/datasource/daily_update_template.xlsx
+++ b/datasource/daily_update_template.xlsx
@@ -1,36 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sindh\datasource\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A0AD0B-2E3C-4B20-B063-A116D21C61C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="stores" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="products" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="inventory" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="daily_update" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>store_id</t>
+  </si>
+  <si>
+    <t>supplier_name</t>
+  </si>
+  <si>
+    <t>stock_days</t>
+  </si>
+  <si>
+    <t>style_code</t>
+  </si>
+  <si>
+    <t>Department_name</t>
+  </si>
+  <si>
+    <t>category_name</t>
+  </si>
+  <si>
+    <t>item_mrp</t>
+  </si>
+  <si>
+    <t>CBS_QTY</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,80 +80,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -410,151 +382,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>city</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>store_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>style_code</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>barcode</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>article_name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>supplier_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>mrp</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>store_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>product_id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>quantity</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>cost_price</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>current_price</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>lifecycle_start_date</t>
-        </is>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sync all current changes
</commit_message>
<xml_diff>
--- a/datasource/daily_update_template.xlsx
+++ b/datasource/daily_update_template.xlsx
@@ -1,67 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sindh\datasource\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A0AD0B-2E3C-4B20-B063-A116D21C61C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="daily_update" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="daily_update" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>store_id</t>
-  </si>
-  <si>
-    <t>supplier_name</t>
-  </si>
-  <si>
-    <t>stock_days</t>
-  </si>
-  <si>
-    <t>style_code</t>
-  </si>
-  <si>
-    <t>Department_name</t>
-  </si>
-  <si>
-    <t>category_name</t>
-  </si>
-  <si>
-    <t>item_mrp</t>
-  </si>
-  <si>
-    <t>CBS_QTY</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -80,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -382,49 +407,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" customWidth="1"/>
-    <col min="8" max="8" width="20.88671875" customWidth="1"/>
+    <col width="18.5546875" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="22.5546875" customWidth="1" min="4" max="4"/>
+    <col width="17.77734375" customWidth="1" min="5" max="5"/>
+    <col width="20.6640625" customWidth="1" min="6" max="6"/>
+    <col width="19.33203125" customWidth="1" min="7" max="7"/>
+    <col width="20.88671875" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>store_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>supplier_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>stock_days</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>style_code</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Department_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>category_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>item_mrp</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>CBS_QTY</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>